<commit_message>
Updated with cell control & protection
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeitrheim\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeitrheim\Documents\Vertice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C88E279B-AE1E-4585-A43C-F9AB00492EA5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA60C661-66BB-4F51-BDFE-BD685732EE48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32730" yWindow="9795" windowWidth="22890" windowHeight="3675" xr2:uid="{717DFAA3-7B66-4F29-9F39-BAA921B8431C}"/>
+    <workbookView xWindow="58260" yWindow="8190" windowWidth="13830" windowHeight="7170" xr2:uid="{717DFAA3-7B66-4F29-9F39-BAA921B8431C}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="150">
   <si>
     <t>Branded</t>
   </si>
@@ -478,6 +478,12 @@
   </si>
   <si>
     <t>R&amp;D Infrastructure Cost ($mil):</t>
+  </si>
+  <si>
+    <t>Is this needed?</t>
+  </si>
+  <si>
+    <t>password: Vertice</t>
   </si>
 </sst>
 </file>
@@ -676,7 +682,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -712,88 +718,140 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="5" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1114,7 +1172,7 @@
   <dimension ref="A1:O98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,196 +1230,203 @@
       <c r="A4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="J4" s="38" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="J4" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="J5" s="43" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="J5" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="J6" s="42" t="s">
+      <c r="B6" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="J6" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="J7" s="34" t="s">
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="J7" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="J8" s="44" t="s">
+      <c r="B8" s="36"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="J8" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="K8" s="45"/>
-      <c r="L8" s="46"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="27"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="J9" s="39" t="s">
+      <c r="B9" s="36"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="J9" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="K9" s="40"/>
-      <c r="L9" s="41"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="33"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="51">
-        <v>4</v>
-      </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="B11" s="38">
+        <v>5</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="51">
+      <c r="B12" s="38">
         <v>2020</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="J13" s="62" t="s">
+        <v>149</v>
+      </c>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="B17" s="50">
+      <c r="B17" s="40">
         <v>1</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1379,81 +1444,81 @@
       <c r="A21" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="52">
-        <v>0</v>
-      </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
+      <c r="B22" s="41">
+        <v>0</v>
+      </c>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="52">
-        <v>0</v>
-      </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
+      <c r="B23" s="41">
+        <v>0</v>
+      </c>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="52">
-        <v>0</v>
-      </c>
-      <c r="C24" s="33" t="s">
+      <c r="B24" s="41">
+        <v>0</v>
+      </c>
+      <c r="C24" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="52">
-        <v>0</v>
-      </c>
-      <c r="C25" s="33" t="s">
+      <c r="B25" s="41">
+        <v>0</v>
+      </c>
+      <c r="C25" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
       <c r="H25" s="6"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="21">
+      <c r="B26" s="20">
         <f>SUM(B24:B25)</f>
         <v>0</v>
       </c>
-      <c r="C26" s="35"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="37"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="45"/>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1467,124 +1532,124 @@
       <c r="A30" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="54">
-        <v>0</v>
-      </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
+      <c r="B31" s="46">
+        <v>0</v>
+      </c>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="54">
-        <v>0</v>
-      </c>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
+      <c r="B32" s="46">
+        <v>0</v>
+      </c>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="54">
-        <v>0</v>
-      </c>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
+      <c r="B33" s="46">
+        <v>0</v>
+      </c>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="54">
-        <v>0</v>
-      </c>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
+      <c r="B34" s="46">
+        <v>0</v>
+      </c>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="54">
-        <v>0</v>
-      </c>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
+      <c r="B35" s="46">
+        <v>0</v>
+      </c>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="42"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="54">
-        <v>0</v>
-      </c>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
+      <c r="B36" s="46">
+        <v>0</v>
+      </c>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="52">
-        <v>0</v>
-      </c>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="33"/>
+      <c r="B37" s="41">
+        <v>0</v>
+      </c>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="24">
+      <c r="B38" s="47">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C38" s="33" t="s">
+      <c r="C38" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B39" s="26">
+      <c r="B39" s="48">
         <f>2/171.2</f>
         <v>1.1682242990654207E-2</v>
       </c>
-      <c r="C39" s="33" t="s">
+      <c r="C39" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="33"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B40" s="8"/>
@@ -1596,105 +1661,105 @@
       <c r="A42" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B42" s="22"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="19">
+      <c r="B43" s="49">
         <v>60</v>
       </c>
-      <c r="C43" s="33" t="s">
+      <c r="C43" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="D43" s="33"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="B44" s="19">
+      <c r="B44" s="49">
         <v>60</v>
       </c>
-      <c r="C44" s="33" t="s">
+      <c r="C44" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="D44" s="33"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="33"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="19">
+      <c r="B45" s="49">
         <v>30</v>
       </c>
-      <c r="C45" s="33" t="s">
+      <c r="C45" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="42"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B48" s="22"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="35"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="49">
+      <c r="B49" s="50">
         <v>0.15</v>
       </c>
-      <c r="C49" s="33" t="s">
+      <c r="C49" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="D49" s="33"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="33"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="42"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B50" s="49">
+      <c r="B50" s="50">
         <v>0.21</v>
       </c>
-      <c r="C50" s="33" t="s">
+      <c r="C50" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="D50" s="33"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="33"/>
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="19">
+      <c r="B51" s="49">
         <v>7</v>
       </c>
-      <c r="C51" s="33" t="s">
+      <c r="C51" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="D51" s="33"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="33"/>
+      <c r="D51" s="42"/>
+      <c r="E51" s="42"/>
+      <c r="F51" s="42"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B52" s="8"/>
@@ -1721,7 +1786,7 @@
       <c r="A55" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="25">
+      <c r="B55" s="51">
         <v>2019</v>
       </c>
       <c r="C55" s="9">
@@ -1776,85 +1841,85 @@
       <c r="A56" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="B56" s="55">
+      <c r="B56" s="52">
         <v>0.5</v>
       </c>
-      <c r="C56" s="55">
+      <c r="C56" s="52">
         <v>0.5</v>
       </c>
-      <c r="D56" s="55">
+      <c r="D56" s="52">
         <v>0.5</v>
       </c>
-      <c r="E56" s="55">
+      <c r="E56" s="52">
         <v>0.6</v>
       </c>
-      <c r="F56" s="55">
+      <c r="F56" s="52">
         <v>0.6</v>
       </c>
-      <c r="G56" s="55">
+      <c r="G56" s="52">
         <v>0.6</v>
       </c>
-      <c r="H56" s="55">
+      <c r="H56" s="52">
         <v>0.6</v>
       </c>
-      <c r="I56" s="55">
+      <c r="I56" s="52">
         <v>0.7</v>
       </c>
-      <c r="J56" s="55">
+      <c r="J56" s="52">
         <v>0.7</v>
       </c>
-      <c r="K56" s="55">
+      <c r="K56" s="52">
         <v>0.7</v>
       </c>
-      <c r="L56" s="55">
+      <c r="L56" s="52">
         <v>0.8</v>
       </c>
-      <c r="M56" s="55">
+      <c r="M56" s="52">
         <v>1</v>
       </c>
-      <c r="N56" s="30"/>
+      <c r="N56" s="53"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="B57" s="53">
+      <c r="B57" s="54">
         <v>2</v>
       </c>
-      <c r="C57" s="53">
+      <c r="C57" s="54">
         <v>2</v>
       </c>
-      <c r="D57" s="53">
+      <c r="D57" s="54">
         <v>2</v>
       </c>
-      <c r="E57" s="53">
+      <c r="E57" s="54">
         <v>3</v>
       </c>
-      <c r="F57" s="53">
+      <c r="F57" s="54">
         <v>4</v>
       </c>
-      <c r="G57" s="53">
+      <c r="G57" s="54">
         <v>4</v>
       </c>
-      <c r="H57" s="53">
+      <c r="H57" s="54">
         <v>4</v>
       </c>
-      <c r="I57" s="53">
+      <c r="I57" s="54">
         <v>4</v>
       </c>
-      <c r="J57" s="53">
+      <c r="J57" s="54">
         <v>4</v>
       </c>
-      <c r="K57" s="53">
+      <c r="K57" s="54">
         <v>4</v>
       </c>
-      <c r="L57" s="53">
+      <c r="L57" s="54">
         <v>5</v>
       </c>
-      <c r="M57" s="53">
+      <c r="M57" s="54">
         <v>6</v>
       </c>
-      <c r="N57" s="48" t="s">
+      <c r="N57" s="55" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1862,55 +1927,55 @@
       <c r="A58" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="B58" s="55">
+      <c r="B58" s="52">
         <f>HLOOKUP(B57,Analog!$B$1:$L$7,IF($B$7="Retail",2,IF($B$7="Clinic",4,6)))</f>
         <v>0.35</v>
       </c>
-      <c r="C58" s="55">
+      <c r="C58" s="52">
         <f>HLOOKUP(C57,Analog!$B$1:$L$7,IF($B$7="Retail",2,IF($B$7="Clinic",4,6)))</f>
         <v>0.35</v>
       </c>
-      <c r="D58" s="55">
+      <c r="D58" s="52">
         <f>HLOOKUP(D57,Analog!$B$1:$L$7,IF($B$7="Retail",2,IF($B$7="Clinic",4,6)))</f>
         <v>0.35</v>
       </c>
-      <c r="E58" s="55">
+      <c r="E58" s="52">
         <f>HLOOKUP(E57,Analog!$B$1:$L$7,IF($B$7="Retail",2,IF($B$7="Clinic",4,6)))</f>
         <v>0.25</v>
       </c>
-      <c r="F58" s="55">
+      <c r="F58" s="52">
         <f>HLOOKUP(F57,Analog!$B$1:$L$7,IF($B$7="Retail",2,IF($B$7="Clinic",4,6)))</f>
         <v>0.2</v>
       </c>
-      <c r="G58" s="55">
+      <c r="G58" s="52">
         <f>HLOOKUP(G57,Analog!$B$1:$L$7,IF($B$7="Retail",2,IF($B$7="Clinic",4,6)))</f>
         <v>0.2</v>
       </c>
-      <c r="H58" s="55">
+      <c r="H58" s="52">
         <f>HLOOKUP(H57,Analog!$B$1:$L$7,IF($B$7="Retail",2,IF($B$7="Clinic",4,6)))</f>
         <v>0.2</v>
       </c>
-      <c r="I58" s="55">
+      <c r="I58" s="52">
         <f>HLOOKUP(I57,Analog!$B$1:$L$7,IF($B$7="Retail",2,IF($B$7="Clinic",4,6)))</f>
         <v>0.2</v>
       </c>
-      <c r="J58" s="55">
+      <c r="J58" s="52">
         <f>HLOOKUP(J57,Analog!$B$1:$L$7,IF($B$7="Retail",2,IF($B$7="Clinic",4,6)))</f>
         <v>0.2</v>
       </c>
-      <c r="K58" s="55">
+      <c r="K58" s="52">
         <f>HLOOKUP(K57,Analog!$B$1:$L$7,IF($B$7="Retail",2,IF($B$7="Clinic",4,6)))</f>
         <v>0.2</v>
       </c>
-      <c r="L58" s="55">
+      <c r="L58" s="52">
         <f>HLOOKUP(L57,Analog!$B$1:$L$7,IF($B$7="Retail",2,IF($B$7="Clinic",4,6)))</f>
         <v>0.1</v>
       </c>
-      <c r="M58" s="55">
+      <c r="M58" s="52">
         <f>HLOOKUP(M57,Analog!$B$1:$L$7,IF($B$7="Retail",2,IF($B$7="Clinic",4,6)))</f>
         <v>0.05</v>
       </c>
-      <c r="N58" s="48" t="s">
+      <c r="N58" s="55" t="s">
         <v>146</v>
       </c>
     </row>
@@ -1918,43 +1983,43 @@
       <c r="A59" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B59" s="55">
-        <v>0</v>
-      </c>
-      <c r="C59" s="55">
+      <c r="B59" s="52">
+        <v>0</v>
+      </c>
+      <c r="C59" s="52">
         <v>0.1</v>
       </c>
-      <c r="D59" s="55">
+      <c r="D59" s="52">
         <v>0.1</v>
       </c>
-      <c r="E59" s="55">
+      <c r="E59" s="52">
         <v>0.1</v>
       </c>
-      <c r="F59" s="55">
+      <c r="F59" s="52">
         <v>0.1</v>
       </c>
-      <c r="G59" s="55">
+      <c r="G59" s="52">
         <v>0.2</v>
       </c>
-      <c r="H59" s="55">
+      <c r="H59" s="52">
         <v>0.2</v>
       </c>
-      <c r="I59" s="55">
+      <c r="I59" s="52">
         <v>0.3</v>
       </c>
-      <c r="J59" s="55">
+      <c r="J59" s="52">
         <v>0.3</v>
       </c>
-      <c r="K59" s="55">
+      <c r="K59" s="52">
         <v>0.3</v>
       </c>
-      <c r="L59" s="55">
+      <c r="L59" s="52">
         <v>0.4</v>
       </c>
-      <c r="M59" s="55">
+      <c r="M59" s="52">
         <v>0.5</v>
       </c>
-      <c r="N59" s="48" t="s">
+      <c r="N59" s="55" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1962,37 +2027,37 @@
       <c r="A60" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B60" s="47"/>
-      <c r="C60" s="47"/>
-      <c r="D60" s="47"/>
-      <c r="E60" s="47"/>
-      <c r="F60" s="47"/>
-      <c r="G60" s="47"/>
-      <c r="H60" s="47"/>
-      <c r="I60" s="47"/>
-      <c r="J60" s="47"/>
-      <c r="K60" s="47"/>
-      <c r="L60" s="47"/>
-      <c r="M60" s="47"/>
-      <c r="N60" s="48"/>
+      <c r="B60" s="56"/>
+      <c r="C60" s="56"/>
+      <c r="D60" s="56"/>
+      <c r="E60" s="56"/>
+      <c r="F60" s="56"/>
+      <c r="G60" s="56"/>
+      <c r="H60" s="56"/>
+      <c r="I60" s="56"/>
+      <c r="J60" s="56"/>
+      <c r="K60" s="56"/>
+      <c r="L60" s="56"/>
+      <c r="M60" s="56"/>
+      <c r="N60" s="55"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="B61" s="56"/>
-      <c r="C61" s="56"/>
-      <c r="D61" s="56"/>
-      <c r="E61" s="56"/>
-      <c r="F61" s="56"/>
-      <c r="G61" s="56"/>
-      <c r="H61" s="56"/>
-      <c r="I61" s="56"/>
-      <c r="J61" s="56"/>
-      <c r="K61" s="56"/>
-      <c r="L61" s="56"/>
-      <c r="M61" s="56"/>
-      <c r="N61" s="48" t="s">
+      <c r="B61" s="57"/>
+      <c r="C61" s="57"/>
+      <c r="D61" s="57"/>
+      <c r="E61" s="57"/>
+      <c r="F61" s="57"/>
+      <c r="G61" s="57"/>
+      <c r="H61" s="57"/>
+      <c r="I61" s="57"/>
+      <c r="J61" s="57"/>
+      <c r="K61" s="57"/>
+      <c r="L61" s="57"/>
+      <c r="M61" s="57"/>
+      <c r="N61" s="55" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2000,19 +2065,19 @@
       <c r="A62" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="B62" s="56"/>
-      <c r="C62" s="56"/>
-      <c r="D62" s="56"/>
-      <c r="E62" s="56"/>
-      <c r="F62" s="56"/>
-      <c r="G62" s="56"/>
-      <c r="H62" s="56"/>
-      <c r="I62" s="56"/>
-      <c r="J62" s="56"/>
-      <c r="K62" s="56"/>
-      <c r="L62" s="56"/>
-      <c r="M62" s="56"/>
-      <c r="N62" s="48" t="s">
+      <c r="B62" s="57"/>
+      <c r="C62" s="57"/>
+      <c r="D62" s="57"/>
+      <c r="E62" s="57"/>
+      <c r="F62" s="57"/>
+      <c r="G62" s="57"/>
+      <c r="H62" s="57"/>
+      <c r="I62" s="57"/>
+      <c r="J62" s="57"/>
+      <c r="K62" s="57"/>
+      <c r="L62" s="57"/>
+      <c r="M62" s="57"/>
+      <c r="N62" s="55" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2020,19 +2085,19 @@
       <c r="A63" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="B63" s="56"/>
-      <c r="C63" s="56"/>
-      <c r="D63" s="56"/>
-      <c r="E63" s="56"/>
-      <c r="F63" s="56"/>
-      <c r="G63" s="56"/>
-      <c r="H63" s="56"/>
-      <c r="I63" s="56"/>
-      <c r="J63" s="56"/>
-      <c r="K63" s="56"/>
-      <c r="L63" s="56"/>
-      <c r="M63" s="56"/>
-      <c r="N63" s="48" t="s">
+      <c r="B63" s="57"/>
+      <c r="C63" s="57"/>
+      <c r="D63" s="57"/>
+      <c r="E63" s="57"/>
+      <c r="F63" s="57"/>
+      <c r="G63" s="57"/>
+      <c r="H63" s="57"/>
+      <c r="I63" s="57"/>
+      <c r="J63" s="57"/>
+      <c r="K63" s="57"/>
+      <c r="L63" s="57"/>
+      <c r="M63" s="57"/>
+      <c r="N63" s="55" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2040,19 +2105,19 @@
       <c r="A64" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="B64" s="56"/>
-      <c r="C64" s="56"/>
-      <c r="D64" s="56"/>
-      <c r="E64" s="56"/>
-      <c r="F64" s="56"/>
-      <c r="G64" s="56"/>
-      <c r="H64" s="56"/>
-      <c r="I64" s="56"/>
-      <c r="J64" s="56"/>
-      <c r="K64" s="56"/>
-      <c r="L64" s="56"/>
-      <c r="M64" s="56"/>
-      <c r="N64" s="48" t="s">
+      <c r="B64" s="57"/>
+      <c r="C64" s="57"/>
+      <c r="D64" s="57"/>
+      <c r="E64" s="57"/>
+      <c r="F64" s="57"/>
+      <c r="G64" s="57"/>
+      <c r="H64" s="57"/>
+      <c r="I64" s="57"/>
+      <c r="J64" s="57"/>
+      <c r="K64" s="57"/>
+      <c r="L64" s="57"/>
+      <c r="M64" s="57"/>
+      <c r="N64" s="55" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2060,75 +2125,75 @@
       <c r="A65" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="B65" s="56"/>
-      <c r="C65" s="56"/>
-      <c r="D65" s="56"/>
-      <c r="E65" s="56"/>
-      <c r="F65" s="56"/>
-      <c r="G65" s="56"/>
-      <c r="H65" s="56"/>
-      <c r="I65" s="56"/>
-      <c r="J65" s="56"/>
-      <c r="K65" s="56"/>
-      <c r="L65" s="56"/>
-      <c r="M65" s="56"/>
-      <c r="N65" s="48" t="s">
+      <c r="B65" s="57"/>
+      <c r="C65" s="57"/>
+      <c r="D65" s="57"/>
+      <c r="E65" s="57"/>
+      <c r="F65" s="57"/>
+      <c r="G65" s="57"/>
+      <c r="H65" s="57"/>
+      <c r="I65" s="57"/>
+      <c r="J65" s="57"/>
+      <c r="K65" s="57"/>
+      <c r="L65" s="57"/>
+      <c r="M65" s="57"/>
+      <c r="N65" s="55" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A66" s="20" t="s">
+      <c r="A66" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="B66" s="21">
+      <c r="B66" s="20">
         <f>B63+B64+B65</f>
         <v>0</v>
       </c>
-      <c r="C66" s="21">
+      <c r="C66" s="20">
         <f t="shared" ref="C66:M66" si="1">C63+C64+C65</f>
         <v>0</v>
       </c>
-      <c r="D66" s="21">
+      <c r="D66" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E66" s="21">
+      <c r="E66" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F66" s="21">
+      <c r="F66" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G66" s="21">
+      <c r="G66" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H66" s="21">
+      <c r="H66" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I66" s="21">
+      <c r="I66" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J66" s="21">
+      <c r="J66" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K66" s="21">
+      <c r="K66" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L66" s="21">
+      <c r="L66" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M66" s="21">
+      <c r="M66" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N66" s="21"/>
+      <c r="N66" s="20"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="7"/>
@@ -2220,148 +2285,148 @@
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="B71" s="57"/>
-      <c r="C71" s="57"/>
-      <c r="D71" s="57"/>
-      <c r="E71" s="57"/>
-      <c r="F71" s="57"/>
-      <c r="G71" s="57"/>
-      <c r="H71" s="57"/>
-      <c r="I71" s="57"/>
-      <c r="J71" s="57"/>
-      <c r="K71" s="57"/>
-      <c r="L71" s="57"/>
-      <c r="M71" s="57"/>
-      <c r="N71" s="29"/>
+      <c r="B71" s="59"/>
+      <c r="C71" s="59"/>
+      <c r="D71" s="59"/>
+      <c r="E71" s="59"/>
+      <c r="F71" s="59"/>
+      <c r="G71" s="59"/>
+      <c r="H71" s="59"/>
+      <c r="I71" s="59"/>
+      <c r="J71" s="59"/>
+      <c r="K71" s="59"/>
+      <c r="L71" s="59"/>
+      <c r="M71" s="59"/>
+      <c r="N71" s="60"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A72" s="11" t="s">
+      <c r="A72" s="58" t="s">
         <v>132</v>
       </c>
-      <c r="B72" s="57"/>
-      <c r="C72" s="57"/>
-      <c r="D72" s="57"/>
-      <c r="E72" s="57"/>
-      <c r="F72" s="57"/>
-      <c r="G72" s="57"/>
-      <c r="H72" s="57"/>
-      <c r="I72" s="57"/>
-      <c r="J72" s="57"/>
-      <c r="K72" s="57"/>
-      <c r="L72" s="57"/>
-      <c r="M72" s="57"/>
-      <c r="N72" s="29"/>
+      <c r="B72" s="59"/>
+      <c r="C72" s="59"/>
+      <c r="D72" s="59"/>
+      <c r="E72" s="59"/>
+      <c r="F72" s="59"/>
+      <c r="G72" s="59"/>
+      <c r="H72" s="59"/>
+      <c r="I72" s="59"/>
+      <c r="J72" s="59"/>
+      <c r="K72" s="59"/>
+      <c r="L72" s="59"/>
+      <c r="M72" s="59"/>
+      <c r="N72" s="60"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A73" s="11" t="s">
+      <c r="A73" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="B73" s="57"/>
-      <c r="C73" s="57"/>
-      <c r="D73" s="57"/>
-      <c r="E73" s="57"/>
-      <c r="F73" s="57"/>
-      <c r="G73" s="57"/>
-      <c r="H73" s="57"/>
-      <c r="I73" s="57"/>
-      <c r="J73" s="57"/>
-      <c r="K73" s="57"/>
-      <c r="L73" s="57"/>
-      <c r="M73" s="57"/>
-      <c r="N73" s="29"/>
+      <c r="B73" s="59"/>
+      <c r="C73" s="59"/>
+      <c r="D73" s="59"/>
+      <c r="E73" s="59"/>
+      <c r="F73" s="59"/>
+      <c r="G73" s="59"/>
+      <c r="H73" s="59"/>
+      <c r="I73" s="59"/>
+      <c r="J73" s="59"/>
+      <c r="K73" s="59"/>
+      <c r="L73" s="59"/>
+      <c r="M73" s="59"/>
+      <c r="N73" s="60"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A74" s="11" t="s">
+      <c r="A74" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="B74" s="57"/>
-      <c r="C74" s="57"/>
-      <c r="D74" s="57"/>
-      <c r="E74" s="57"/>
-      <c r="F74" s="57"/>
-      <c r="G74" s="57"/>
-      <c r="H74" s="57"/>
-      <c r="I74" s="57"/>
-      <c r="J74" s="57"/>
-      <c r="K74" s="57"/>
-      <c r="L74" s="57"/>
-      <c r="M74" s="57"/>
-      <c r="N74" s="29"/>
+      <c r="B74" s="59"/>
+      <c r="C74" s="59"/>
+      <c r="D74" s="59"/>
+      <c r="E74" s="59"/>
+      <c r="F74" s="59"/>
+      <c r="G74" s="59"/>
+      <c r="H74" s="59"/>
+      <c r="I74" s="59"/>
+      <c r="J74" s="59"/>
+      <c r="K74" s="59"/>
+      <c r="L74" s="59"/>
+      <c r="M74" s="59"/>
+      <c r="N74" s="60"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A75" s="20" t="s">
+      <c r="A75" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="B75" s="58">
+      <c r="B75" s="24">
         <f>SUM(B71:B74)</f>
         <v>0</v>
       </c>
-      <c r="C75" s="58">
+      <c r="C75" s="24">
         <f t="shared" ref="C75:M75" si="2">SUM(C71:C74)</f>
         <v>0</v>
       </c>
-      <c r="D75" s="58">
+      <c r="D75" s="24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E75" s="58">
+      <c r="E75" s="24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F75" s="58">
+      <c r="F75" s="24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G75" s="58">
+      <c r="G75" s="24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H75" s="58">
+      <c r="H75" s="24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I75" s="58">
+      <c r="I75" s="24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J75" s="58">
+      <c r="J75" s="24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K75" s="58">
+      <c r="K75" s="24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L75" s="58">
+      <c r="L75" s="24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M75" s="58">
+      <c r="M75" s="24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N75" s="21"/>
+      <c r="N75" s="20"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B76" s="57"/>
-      <c r="C76" s="57"/>
-      <c r="D76" s="57"/>
-      <c r="E76" s="57"/>
-      <c r="F76" s="57"/>
-      <c r="G76" s="57"/>
-      <c r="H76" s="57"/>
-      <c r="I76" s="57"/>
-      <c r="J76" s="57"/>
-      <c r="K76" s="57"/>
-      <c r="L76" s="57"/>
-      <c r="M76" s="57"/>
-      <c r="N76" s="48" t="s">
+      <c r="B76" s="59"/>
+      <c r="C76" s="59"/>
+      <c r="D76" s="59"/>
+      <c r="E76" s="59"/>
+      <c r="F76" s="59"/>
+      <c r="G76" s="59"/>
+      <c r="H76" s="59"/>
+      <c r="I76" s="59"/>
+      <c r="J76" s="59"/>
+      <c r="K76" s="59"/>
+      <c r="L76" s="59"/>
+      <c r="M76" s="59"/>
+      <c r="N76" s="55" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2441,251 +2506,251 @@
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A80" s="11" t="s">
+      <c r="A80" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="B80" s="57"/>
-      <c r="C80" s="59"/>
-      <c r="D80" s="59"/>
-      <c r="E80" s="59"/>
-      <c r="F80" s="59"/>
-      <c r="G80" s="59"/>
-      <c r="H80" s="59"/>
-      <c r="I80" s="59"/>
-      <c r="J80" s="59"/>
-      <c r="K80" s="59"/>
-      <c r="L80" s="59"/>
-      <c r="M80" s="59"/>
-      <c r="N80" s="48" t="s">
+      <c r="B80" s="59"/>
+      <c r="C80" s="61"/>
+      <c r="D80" s="61"/>
+      <c r="E80" s="61"/>
+      <c r="F80" s="61"/>
+      <c r="G80" s="61"/>
+      <c r="H80" s="61"/>
+      <c r="I80" s="61"/>
+      <c r="J80" s="61"/>
+      <c r="K80" s="61"/>
+      <c r="L80" s="61"/>
+      <c r="M80" s="61"/>
+      <c r="N80" s="55" t="s">
         <v>114</v>
       </c>
       <c r="O80" s="6"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A81" s="11" t="s">
+      <c r="A81" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="B81" s="57"/>
-      <c r="C81" s="59"/>
-      <c r="D81" s="59"/>
-      <c r="E81" s="59"/>
-      <c r="F81" s="59"/>
-      <c r="G81" s="59"/>
-      <c r="H81" s="59"/>
-      <c r="I81" s="59"/>
-      <c r="J81" s="59"/>
-      <c r="K81" s="59"/>
-      <c r="L81" s="59"/>
-      <c r="M81" s="59"/>
-      <c r="N81" s="48" t="s">
+      <c r="B81" s="59"/>
+      <c r="C81" s="61"/>
+      <c r="D81" s="61"/>
+      <c r="E81" s="61"/>
+      <c r="F81" s="61"/>
+      <c r="G81" s="61"/>
+      <c r="H81" s="61"/>
+      <c r="I81" s="61"/>
+      <c r="J81" s="61"/>
+      <c r="K81" s="61"/>
+      <c r="L81" s="61"/>
+      <c r="M81" s="61"/>
+      <c r="N81" s="55" t="s">
         <v>114</v>
       </c>
       <c r="O81" s="6"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A82" s="11" t="s">
+      <c r="A82" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="B82" s="57"/>
-      <c r="C82" s="59"/>
-      <c r="D82" s="59"/>
-      <c r="E82" s="59"/>
-      <c r="F82" s="59"/>
-      <c r="G82" s="59"/>
-      <c r="H82" s="59"/>
-      <c r="I82" s="59"/>
-      <c r="J82" s="59"/>
-      <c r="K82" s="59"/>
-      <c r="L82" s="59"/>
-      <c r="M82" s="59"/>
-      <c r="N82" s="48" t="s">
+      <c r="B82" s="59"/>
+      <c r="C82" s="61"/>
+      <c r="D82" s="61"/>
+      <c r="E82" s="61"/>
+      <c r="F82" s="61"/>
+      <c r="G82" s="61"/>
+      <c r="H82" s="61"/>
+      <c r="I82" s="61"/>
+      <c r="J82" s="61"/>
+      <c r="K82" s="61"/>
+      <c r="L82" s="61"/>
+      <c r="M82" s="61"/>
+      <c r="N82" s="55" t="s">
         <v>114</v>
       </c>
       <c r="O82" s="6"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A83" s="11" t="s">
+      <c r="A83" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="B83" s="57"/>
-      <c r="C83" s="59"/>
-      <c r="D83" s="59"/>
-      <c r="E83" s="59"/>
-      <c r="F83" s="59"/>
-      <c r="G83" s="59"/>
-      <c r="H83" s="59"/>
-      <c r="I83" s="59"/>
-      <c r="J83" s="59"/>
-      <c r="K83" s="59"/>
-      <c r="L83" s="59"/>
-      <c r="M83" s="59"/>
-      <c r="N83" s="48" t="s">
+      <c r="B83" s="59"/>
+      <c r="C83" s="61"/>
+      <c r="D83" s="61"/>
+      <c r="E83" s="61"/>
+      <c r="F83" s="61"/>
+      <c r="G83" s="61"/>
+      <c r="H83" s="61"/>
+      <c r="I83" s="61"/>
+      <c r="J83" s="61"/>
+      <c r="K83" s="61"/>
+      <c r="L83" s="61"/>
+      <c r="M83" s="61"/>
+      <c r="N83" s="55" t="s">
         <v>114</v>
       </c>
       <c r="O83" s="6"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A84" s="20" t="s">
+      <c r="A84" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="B84" s="58">
+      <c r="B84" s="24">
         <f>SUM(B80:B83)</f>
         <v>0</v>
       </c>
-      <c r="C84" s="58">
+      <c r="C84" s="24">
         <f t="shared" ref="C84:M84" si="3">SUM(C80:C83)</f>
         <v>0</v>
       </c>
-      <c r="D84" s="58">
+      <c r="D84" s="24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E84" s="58">
+      <c r="E84" s="24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F84" s="58">
+      <c r="F84" s="24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G84" s="58">
+      <c r="G84" s="24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H84" s="58">
+      <c r="H84" s="24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I84" s="58">
+      <c r="I84" s="24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J84" s="58">
+      <c r="J84" s="24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K84" s="58">
+      <c r="K84" s="24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L84" s="58">
+      <c r="L84" s="24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M84" s="58">
+      <c r="M84" s="24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N84" s="21"/>
+      <c r="N84" s="20"/>
       <c r="O84" s="6"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B85" s="57"/>
-      <c r="C85" s="57"/>
-      <c r="D85" s="57"/>
-      <c r="E85" s="57"/>
-      <c r="F85" s="57"/>
-      <c r="G85" s="57"/>
-      <c r="H85" s="57"/>
-      <c r="I85" s="57"/>
-      <c r="J85" s="57"/>
-      <c r="K85" s="57"/>
-      <c r="L85" s="57"/>
-      <c r="M85" s="57"/>
-      <c r="N85" s="29"/>
-    </row>
-    <row r="86" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B85" s="59"/>
+      <c r="C85" s="59"/>
+      <c r="D85" s="59"/>
+      <c r="E85" s="59"/>
+      <c r="F85" s="59"/>
+      <c r="G85" s="59"/>
+      <c r="H85" s="59"/>
+      <c r="I85" s="59"/>
+      <c r="J85" s="59"/>
+      <c r="K85" s="59"/>
+      <c r="L85" s="59"/>
+      <c r="M85" s="59"/>
+      <c r="N85" s="60"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B86" s="57"/>
-      <c r="C86" s="57"/>
-      <c r="D86" s="57"/>
-      <c r="E86" s="57"/>
-      <c r="F86" s="57"/>
-      <c r="G86" s="57"/>
-      <c r="H86" s="57"/>
-      <c r="I86" s="57"/>
-      <c r="J86" s="57"/>
-      <c r="K86" s="57"/>
-      <c r="L86" s="57"/>
-      <c r="M86" s="57"/>
-      <c r="N86" s="29"/>
+      <c r="B86" s="59"/>
+      <c r="C86" s="59"/>
+      <c r="D86" s="59"/>
+      <c r="E86" s="59"/>
+      <c r="F86" s="59"/>
+      <c r="G86" s="59"/>
+      <c r="H86" s="59"/>
+      <c r="I86" s="59"/>
+      <c r="J86" s="59"/>
+      <c r="K86" s="59"/>
+      <c r="L86" s="59"/>
+      <c r="M86" s="59"/>
+      <c r="N86" s="60"/>
     </row>
     <row r="87" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B87" s="57"/>
-      <c r="C87" s="57"/>
-      <c r="D87" s="57"/>
-      <c r="E87" s="57"/>
-      <c r="F87" s="57"/>
-      <c r="G87" s="57"/>
-      <c r="H87" s="57"/>
-      <c r="I87" s="57"/>
-      <c r="J87" s="57"/>
-      <c r="K87" s="57"/>
-      <c r="L87" s="57"/>
-      <c r="M87" s="57"/>
-      <c r="N87" s="29"/>
+      <c r="B87" s="59"/>
+      <c r="C87" s="59"/>
+      <c r="D87" s="59"/>
+      <c r="E87" s="59"/>
+      <c r="F87" s="59"/>
+      <c r="G87" s="59"/>
+      <c r="H87" s="59"/>
+      <c r="I87" s="59"/>
+      <c r="J87" s="59"/>
+      <c r="K87" s="59"/>
+      <c r="L87" s="59"/>
+      <c r="M87" s="59"/>
+      <c r="N87" s="60"/>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B88" s="57"/>
-      <c r="C88" s="57"/>
-      <c r="D88" s="57"/>
-      <c r="E88" s="57"/>
-      <c r="F88" s="57"/>
-      <c r="G88" s="57"/>
-      <c r="H88" s="57"/>
-      <c r="I88" s="57"/>
-      <c r="J88" s="57"/>
-      <c r="K88" s="57"/>
-      <c r="L88" s="57"/>
-      <c r="M88" s="57"/>
-      <c r="N88" s="29"/>
+      <c r="B88" s="59"/>
+      <c r="C88" s="59"/>
+      <c r="D88" s="59"/>
+      <c r="E88" s="59"/>
+      <c r="F88" s="59"/>
+      <c r="G88" s="59"/>
+      <c r="H88" s="59"/>
+      <c r="I88" s="59"/>
+      <c r="J88" s="59"/>
+      <c r="K88" s="59"/>
+      <c r="L88" s="59"/>
+      <c r="M88" s="59"/>
+      <c r="N88" s="60"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B89" s="57"/>
-      <c r="C89" s="57"/>
-      <c r="D89" s="57"/>
-      <c r="E89" s="57"/>
-      <c r="F89" s="57"/>
-      <c r="G89" s="57"/>
-      <c r="H89" s="57"/>
-      <c r="I89" s="57"/>
-      <c r="J89" s="57"/>
-      <c r="K89" s="57"/>
-      <c r="L89" s="57"/>
-      <c r="M89" s="57"/>
-      <c r="N89" s="29"/>
+      <c r="B89" s="59"/>
+      <c r="C89" s="59"/>
+      <c r="D89" s="59"/>
+      <c r="E89" s="59"/>
+      <c r="F89" s="59"/>
+      <c r="G89" s="59"/>
+      <c r="H89" s="59"/>
+      <c r="I89" s="59"/>
+      <c r="J89" s="59"/>
+      <c r="K89" s="59"/>
+      <c r="L89" s="59"/>
+      <c r="M89" s="59"/>
+      <c r="N89" s="60"/>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B90" s="57"/>
-      <c r="C90" s="57"/>
-      <c r="D90" s="57"/>
-      <c r="E90" s="57"/>
-      <c r="F90" s="57"/>
-      <c r="G90" s="57"/>
-      <c r="H90" s="57"/>
-      <c r="I90" s="57"/>
-      <c r="J90" s="57"/>
-      <c r="K90" s="57"/>
-      <c r="L90" s="57"/>
-      <c r="M90" s="57"/>
-      <c r="N90" s="29"/>
+      <c r="B90" s="59"/>
+      <c r="C90" s="59"/>
+      <c r="D90" s="59"/>
+      <c r="E90" s="59"/>
+      <c r="F90" s="59"/>
+      <c r="G90" s="59"/>
+      <c r="H90" s="59"/>
+      <c r="I90" s="59"/>
+      <c r="J90" s="59"/>
+      <c r="K90" s="59"/>
+      <c r="L90" s="59"/>
+      <c r="M90" s="59"/>
+      <c r="N90" s="60"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" s="7"/>
@@ -2701,48 +2766,12 @@
       <c r="L91" s="6"/>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" s="27"/>
+      <c r="A98" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="C42:F42"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C39:F39"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2Otz3bK7/G61JqKDFCxF+3XYx/82ahsdKVgeWax4Q5ttOplclDt0WU2Zsm/gYpCwMoDjCTZx2kUlAwxCF+T8UQ==" saltValue="D1xBYV6tZcRfmXYvePYy+w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="46">
+    <mergeCell ref="J13:L13"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C5:F5"/>
@@ -2750,10 +2779,48 @@
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C39:F39"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C42:F42"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J6:L6"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11 B9" xr:uid="{FB8FC8F8-FB3B-423C-85F6-7C30F382E001}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9 B11" xr:uid="{FB8FC8F8-FB3B-423C-85F6-7C30F382E001}">
       <formula1>1</formula1>
       <formula2>12</formula2>
     </dataValidation>
@@ -2805,7 +2872,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="23" t="s">
         <v>122</v>
       </c>
       <c r="B1">

</xml_diff>